<commit_message>
Add Laboratory Tests export for AB#12267.
</commit_message>
<xml_diff>
--- a/Apps/WebClient/src/Server/Assets/Templates/LaboratoryReport.xlsx
+++ b/Apps/WebClient/src/Server/Assets/Templates/LaboratoryReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_bugs\Apps\WebClient\src\Server\Assets\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianjang/Repo/healthgateway/Apps/WebClient/src/Server/Assets/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DEF8A7-3B6F-4F53-B257-39017DBFBC92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33C03C2-7397-4D44-A565-80D3423677DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
+    <workbookView xWindow="-43020" yWindow="2640" windowWidth="34560" windowHeight="21580" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,22 +54,22 @@
     <t>Status</t>
   </si>
   <si>
-    <t>{d.records[i].collectionDateTime}</t>
-  </si>
-  <si>
-    <t>{d.records[i+1].collectionDateTime}</t>
-  </si>
-  <si>
-    <t>{d.records[i].batteryType}</t>
-  </si>
-  <si>
-    <t>{d.records[i+1].batteryType}</t>
-  </si>
-  <si>
-    <t>{d.records[i].testStatus}</t>
-  </si>
-  <si>
-    <t>{d.records[i+1].testStatus}</t>
+    <t>{d.records[i].date}</t>
+  </si>
+  <si>
+    <t>{d.records[i+1].date}</t>
+  </si>
+  <si>
+    <t>{d.records[i].test}</t>
+  </si>
+  <si>
+    <t>{d.records[i+1].test}</t>
+  </si>
+  <si>
+    <t>{d.records[i].status}</t>
+  </si>
+  <si>
+    <t>{d.records[i+1].status}</t>
   </si>
 </sst>
 </file>
@@ -446,19 +446,19 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.09765625" customWidth="1"/>
-    <col min="2" max="5" width="35.796875" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="5" width="35.83203125" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="30.796875" customWidth="1"/>
-    <col min="9" max="9" width="44.19921875" customWidth="1"/>
+    <col min="8" max="8" width="30.83203125" customWidth="1"/>
+    <col min="9" max="9" width="44.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -477,7 +477,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -491,7 +491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Add Laboratory Tests export for AB#12267.  (#3254)
* Add Laboratory Tests export for AB#12267.

* Code review and unit test changes for AB#12267.
</commit_message>
<xml_diff>
--- a/Apps/WebClient/src/Server/Assets/Templates/LaboratoryReport.xlsx
+++ b/Apps/WebClient/src/Server/Assets/Templates/LaboratoryReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_bugs\Apps\WebClient\src\Server\Assets\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianjang/Repo/healthgateway/Apps/WebClient/src/Server/Assets/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DEF8A7-3B6F-4F53-B257-39017DBFBC92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33C03C2-7397-4D44-A565-80D3423677DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
+    <workbookView xWindow="-43020" yWindow="2640" windowWidth="34560" windowHeight="21580" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,22 +54,22 @@
     <t>Status</t>
   </si>
   <si>
-    <t>{d.records[i].collectionDateTime}</t>
-  </si>
-  <si>
-    <t>{d.records[i+1].collectionDateTime}</t>
-  </si>
-  <si>
-    <t>{d.records[i].batteryType}</t>
-  </si>
-  <si>
-    <t>{d.records[i+1].batteryType}</t>
-  </si>
-  <si>
-    <t>{d.records[i].testStatus}</t>
-  </si>
-  <si>
-    <t>{d.records[i+1].testStatus}</t>
+    <t>{d.records[i].date}</t>
+  </si>
+  <si>
+    <t>{d.records[i+1].date}</t>
+  </si>
+  <si>
+    <t>{d.records[i].test}</t>
+  </si>
+  <si>
+    <t>{d.records[i+1].test}</t>
+  </si>
+  <si>
+    <t>{d.records[i].status}</t>
+  </si>
+  <si>
+    <t>{d.records[i+1].status}</t>
   </si>
 </sst>
 </file>
@@ -446,19 +446,19 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.09765625" customWidth="1"/>
-    <col min="2" max="5" width="35.796875" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="5" width="35.83203125" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="30.796875" customWidth="1"/>
-    <col min="9" max="9" width="44.19921875" customWidth="1"/>
+    <col min="8" max="8" width="30.83203125" customWidth="1"/>
+    <col min="9" max="9" width="44.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -477,7 +477,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -491,7 +491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>

</xml_diff>